<commit_message>
New Script for testing
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Master\FALL_2023\ECE-6654-NENR\ResearchPjt3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\NENR_Project3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D9C3BB-22E7-4339-A724-54A6BA2AC34A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB082C1-57CC-4DEB-8C88-E0F64C922976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -468,12 +468,12 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Data gathered 10-27, 18:03
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20403"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\NENR_Project3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\chips.eng.utah.edu\home\u0912711\.win_my_documents\ECE 6654\NENR_Project3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB082C1-57CC-4DEB-8C88-E0F64C922976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4B6B99-A86D-4924-8D11-3F98152DD38B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t xml:space="preserve">Output Characteristic Device </t>
   </si>
@@ -135,9 +135,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Burs</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -145,6 +142,36 @@
   </si>
   <si>
     <t>interleaved biphasic pulses</t>
+  </si>
+  <si>
+    <t>Voltage Regulated</t>
+  </si>
+  <si>
+    <t>Current / pulse width</t>
+  </si>
+  <si>
+    <t>Peak voltage / resistance</t>
+  </si>
+  <si>
+    <t>Max volt peak/510- min volt/510</t>
+  </si>
+  <si>
+    <t>Use cell B17 and divide by elerode area</t>
+  </si>
+  <si>
+    <t>Burst</t>
+  </si>
+  <si>
+    <t>240hz, 250 uS, 1 mA</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>30-240</t>
+  </si>
+  <si>
+    <t>Biphasic symmetrical</t>
   </si>
 </sst>
 </file>
@@ -465,159 +492,217 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <f>0.001*510</f>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>2.5000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14">
+        <f>((0.862-0.532)/510)*10^9</f>
+        <v>647058.82352941169</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15">
+        <f>((0.532-0.528)/510)*10^6</f>
+        <v>7.8431372549019676</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="B16" s="1">
+        <f>(0.532/510)*(250/(10^6))</f>
+        <v>2.6078431372549019E-7</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="B17" s="1"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
+      <c r="B18" s="1">
+        <f>0.532*(0.001)</f>
+        <v>5.3200000000000003E-4</v>
+      </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>30</v>
+      <c r="B20" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B21" s="1"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B22" s="1"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="B23" s="1"/>
     </row>
     <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -625,8 +710,8 @@
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B25" t="s">
-        <v>31</v>
+      <c r="B25" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>